<commit_message>
Add LLM validation pipeline with Azure OpenAI integration
- Integrated `run_llm_validation` module using Azure OpenAI GPT-4o
- Wrote results to both JSONL and flattened CSV formats
- Refactored CSV writing logic into `utilities/file_utils.py` (write_json_to_csv)
- Updated config.yaml to include LLM input/output paths
- Cleaned up unused config loading logic in llm_validator.py
- Validated entire pipeline end-to-end via main.py
</commit_message>
<xml_diff>
--- a/sample_data/input/sample_vendor_data.xlsx
+++ b/sample_data/input/sample_vendor_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyFiles\ER\ta_entity_resolver\sample_data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7E7A8F-9511-4837-8936-B6DED90BB8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178204A1-259F-44E0-98E5-09CF54EE4588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{9152D6CB-B07D-479D-B42B-6A26789F2475}"/>
+    <workbookView xWindow="83" yWindow="450" windowWidth="28717" windowHeight="15030" xr2:uid="{9152D6CB-B07D-479D-B42B-6A26789F2475}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Raw_Vendor_Name</t>
   </si>
@@ -965,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C708708C-4D46-4B90-B415-5AD946F0D5FF}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1081,6 +1081,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>